<commit_message>
Clustering by environmental variables
</commit_message>
<xml_diff>
--- a/SP_metadata_2021.xlsx
+++ b/SP_metadata_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugirona-my.sharepoint.com/personal/u4001033_udg_edu/Documents/GRADCATCH/ANALISIS/R/SP_gradient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{4EEA8018-6EF8-42D3-98FB-882912627FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2004EE7-2EC7-45C3-9B98-8EEB917BF82B}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{4EEA8018-6EF8-42D3-98FB-882912627FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E8D6EF0-F84F-4D19-A880-D9E76097A7B7}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3072" yWindow="720" windowWidth="18360" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP_soil_2021" sheetId="1" r:id="rId1"/>
@@ -1875,10 +1875,10 @@
   <dimension ref="A1:BZ61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AW29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:B61"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2153,7 +2153,7 @@
       <c r="F2" s="5">
         <v>12.13822558</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="7">
         <v>1.248428493</v>
       </c>
       <c r="H2" s="5">
@@ -2402,7 +2402,7 @@
       <c r="F3" s="5">
         <v>12.13822558</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="7">
         <v>1.248428493</v>
       </c>
       <c r="H3" s="5">
@@ -2651,7 +2651,7 @@
       <c r="F4" s="5">
         <v>12.13822558</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="7">
         <v>1.248428493</v>
       </c>
       <c r="H4" s="5">
@@ -2900,7 +2900,7 @@
       <c r="F5" s="5">
         <v>12.13822558</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="7">
         <v>1.248428493</v>
       </c>
       <c r="H5" s="5">
@@ -3141,7 +3141,7 @@
       <c r="F6" s="5">
         <v>12.13822558</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="7">
         <v>1.248428493</v>
       </c>
       <c r="H6" s="5">
@@ -3388,7 +3388,7 @@
       <c r="F7" s="5">
         <v>10.970743150000001</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="7">
         <v>1.0879099809999999</v>
       </c>
       <c r="H7" s="5">
@@ -3638,7 +3638,7 @@
       <c r="F8" s="5">
         <v>10.970743150000001</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="7">
         <v>1.0879099809999999</v>
       </c>
       <c r="H8" s="5">
@@ -3888,7 +3888,7 @@
       <c r="F9" s="5">
         <v>10.970743150000001</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="7">
         <v>1.0879099809999999</v>
       </c>
       <c r="H9" s="5">
@@ -4138,7 +4138,7 @@
       <c r="F10" s="5">
         <v>10.970743150000001</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="7">
         <v>1.0879099809999999</v>
       </c>
       <c r="H10" s="5">
@@ -4388,7 +4388,7 @@
       <c r="F11" s="5">
         <v>10.970743150000001</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="7">
         <v>1.0879099809999999</v>
       </c>
       <c r="H11" s="5">
@@ -4636,7 +4636,7 @@
       <c r="F12" s="5">
         <v>13.84807052</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="7">
         <v>0.56437017</v>
       </c>
       <c r="H12" s="5">
@@ -4885,7 +4885,7 @@
       <c r="F13" s="5">
         <v>13.84807052</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="7">
         <v>0.56437017</v>
       </c>
       <c r="H13" s="5">
@@ -5126,7 +5126,7 @@
       <c r="F14" s="5">
         <v>13.84807052</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="7">
         <v>0.56437017</v>
       </c>
       <c r="H14" s="5">
@@ -5375,7 +5375,7 @@
       <c r="F15" s="5">
         <v>13.84807052</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="7">
         <v>0.56437017</v>
       </c>
       <c r="H15" s="5">
@@ -5624,7 +5624,7 @@
       <c r="F16" s="5">
         <v>13.84807052</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="7">
         <v>0.56437017</v>
       </c>
       <c r="H16" s="5">
@@ -5873,7 +5873,7 @@
       <c r="F17" s="5">
         <v>13.479537779999999</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="7">
         <v>0.24611151000000001</v>
       </c>
       <c r="H17" s="5">
@@ -6122,7 +6122,7 @@
       <c r="F18" s="5">
         <v>13.479537779999999</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="7">
         <v>0.24611151000000001</v>
       </c>
       <c r="H18" s="5">
@@ -6371,7 +6371,7 @@
       <c r="F19" s="5">
         <v>13.479537779999999</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="7">
         <v>0.24611151000000001</v>
       </c>
       <c r="H19" s="5">
@@ -6620,7 +6620,7 @@
       <c r="F20" s="5">
         <v>13.479537779999999</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="7">
         <v>0.24611151000000001</v>
       </c>
       <c r="H20" s="5">
@@ -6869,7 +6869,7 @@
       <c r="F21" s="5">
         <v>13.479537779999999</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="7">
         <v>0.24611151000000001</v>
       </c>
       <c r="H21" s="5">
@@ -7110,7 +7110,7 @@
       <c r="F22" s="5">
         <v>16.980182540000001</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="7">
         <v>0.15639571399999999</v>
       </c>
       <c r="H22" s="5">
@@ -7359,7 +7359,7 @@
       <c r="F23" s="5">
         <v>16.980182540000001</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="7">
         <v>0.15639571399999999</v>
       </c>
       <c r="H23" s="5">
@@ -7608,7 +7608,7 @@
       <c r="F24" s="5">
         <v>16.980182540000001</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="7">
         <v>0.15639571399999999</v>
       </c>
       <c r="H24" s="5">
@@ -7857,7 +7857,7 @@
       <c r="F25" s="5">
         <v>16.980182540000001</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="7">
         <v>0.15639571399999999</v>
       </c>
       <c r="H25" s="5">
@@ -8086,7 +8086,7 @@
       <c r="F26" s="5">
         <v>16.980182540000001</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="7">
         <v>0.15639571399999999</v>
       </c>
       <c r="H26" s="5">
@@ -8335,7 +8335,7 @@
       <c r="F27" s="5">
         <v>9.191429608</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="7">
         <v>0.70398598999999995</v>
       </c>
       <c r="H27" s="5">
@@ -8584,7 +8584,7 @@
       <c r="F28" s="5">
         <v>9.191429608</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="7">
         <v>0.70398598999999995</v>
       </c>
       <c r="H28" s="5">
@@ -8825,7 +8825,7 @@
       <c r="F29" s="5">
         <v>9.191429608</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="7">
         <v>0.70398598999999995</v>
       </c>
       <c r="H29" s="5">
@@ -9074,7 +9074,7 @@
       <c r="F30" s="5">
         <v>9.191429608</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="7">
         <v>0.70398598999999995</v>
       </c>
       <c r="H30" s="5">
@@ -9323,7 +9323,7 @@
       <c r="F31" s="5">
         <v>9.191429608</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="7">
         <v>0.70398598999999995</v>
       </c>
       <c r="H31" s="5">
@@ -9572,7 +9572,7 @@
       <c r="F32" s="5">
         <v>9.4308277250000003</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="7">
         <v>0.99706098099999996</v>
       </c>
       <c r="H32" s="5">
@@ -9821,7 +9821,7 @@
       <c r="F33" s="5">
         <v>9.4308277250000003</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="7">
         <v>0.99706098099999996</v>
       </c>
       <c r="H33" s="5">
@@ -10070,7 +10070,7 @@
       <c r="F34" s="5">
         <v>9.4308277250000003</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="7">
         <v>0.99706098099999996</v>
       </c>
       <c r="H34" s="5">
@@ -10319,7 +10319,7 @@
       <c r="F35" s="5">
         <v>9.4308277250000003</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="7">
         <v>0.99706098099999996</v>
       </c>
       <c r="H35" s="5">
@@ -10568,7 +10568,7 @@
       <c r="F36" s="5">
         <v>9.4308277250000003</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="7">
         <v>0.99706098099999996</v>
       </c>
       <c r="H36" s="5">
@@ -10815,7 +10815,7 @@
       <c r="F37" s="5">
         <v>12.17788356</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="7">
         <v>1.3318448700000001</v>
       </c>
       <c r="H37" s="5">
@@ -11064,7 +11064,7 @@
       <c r="F38" s="5">
         <v>12.17788356</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="7">
         <v>1.3318448700000001</v>
       </c>
       <c r="H38" s="5">
@@ -11313,7 +11313,7 @@
       <c r="F39" s="5">
         <v>12.17788356</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="7">
         <v>1.3318448700000001</v>
       </c>
       <c r="H39" s="5">
@@ -11562,7 +11562,7 @@
       <c r="F40" s="5">
         <v>12.17788356</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="7">
         <v>1.3318448700000001</v>
       </c>
       <c r="H40" s="5">
@@ -11811,7 +11811,7 @@
       <c r="F41" s="5">
         <v>12.17788356</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="7">
         <v>1.3318448700000001</v>
       </c>
       <c r="H41" s="5">
@@ -12050,7 +12050,7 @@
       <c r="F42" s="5">
         <v>17.095476130000002</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="7">
         <v>0.184624183</v>
       </c>
       <c r="H42" s="5">
@@ -12299,7 +12299,7 @@
       <c r="F43" s="5">
         <v>17.095476130000002</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G43" s="7">
         <v>0.184624183</v>
       </c>
       <c r="H43" s="5">
@@ -12545,7 +12545,7 @@
       <c r="F44" s="5">
         <v>17.095476130000002</v>
       </c>
-      <c r="G44" s="5">
+      <c r="G44" s="7">
         <v>0.184624183</v>
       </c>
       <c r="H44" s="5">
@@ -12794,7 +12794,7 @@
       <c r="F45" s="5">
         <v>17.095476130000002</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G45" s="7">
         <v>0.184624183</v>
       </c>
       <c r="H45" s="5">
@@ -13043,7 +13043,7 @@
       <c r="F46" s="5">
         <v>17.095476130000002</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G46" s="7">
         <v>0.184624183</v>
       </c>
       <c r="H46" s="5">
@@ -13286,7 +13286,7 @@
       <c r="F47" s="5">
         <v>16.864897020000001</v>
       </c>
-      <c r="G47" s="5">
+      <c r="G47" s="7">
         <v>0.17709229000000001</v>
       </c>
       <c r="H47" s="5">
@@ -13535,7 +13535,7 @@
       <c r="F48" s="5">
         <v>16.864897020000001</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G48" s="7">
         <v>0.17709229000000001</v>
       </c>
       <c r="H48" s="5">
@@ -13784,7 +13784,7 @@
       <c r="F49" s="5">
         <v>16.864897020000001</v>
       </c>
-      <c r="G49" s="5">
+      <c r="G49" s="7">
         <v>0.17709229000000001</v>
       </c>
       <c r="H49" s="5">
@@ -14025,7 +14025,7 @@
       <c r="F50" s="5">
         <v>16.864897020000001</v>
       </c>
-      <c r="G50" s="5">
+      <c r="G50" s="7">
         <v>0.17709229000000001</v>
       </c>
       <c r="H50" s="5">
@@ -14274,7 +14274,7 @@
       <c r="F51" s="5">
         <v>16.864897020000001</v>
       </c>
-      <c r="G51" s="5">
+      <c r="G51" s="7">
         <v>0.17709229000000001</v>
       </c>
       <c r="H51" s="5">
@@ -14523,7 +14523,7 @@
       <c r="F52" s="5">
         <v>14.68688395</v>
       </c>
-      <c r="G52" s="5">
+      <c r="G52" s="7">
         <v>0.40075582599999998</v>
       </c>
       <c r="H52" s="5">
@@ -14772,7 +14772,7 @@
       <c r="F53" s="5">
         <v>14.68688395</v>
       </c>
-      <c r="G53" s="5">
+      <c r="G53" s="7">
         <v>0.40075582599999998</v>
       </c>
       <c r="H53" s="5">
@@ -15021,7 +15021,7 @@
       <c r="F54" s="5">
         <v>14.68688395</v>
       </c>
-      <c r="G54" s="5">
+      <c r="G54" s="7">
         <v>0.40075582599999998</v>
       </c>
       <c r="H54" s="5">
@@ -15270,7 +15270,7 @@
       <c r="F55" s="5">
         <v>14.68688395</v>
       </c>
-      <c r="G55" s="5">
+      <c r="G55" s="7">
         <v>0.40075582599999998</v>
       </c>
       <c r="H55" s="5">
@@ -15504,7 +15504,7 @@
       <c r="F56" s="5">
         <v>14.68688395</v>
       </c>
-      <c r="G56" s="5">
+      <c r="G56" s="7">
         <v>0.40075582599999998</v>
       </c>
       <c r="H56" s="5">
@@ -15753,7 +15753,7 @@
       <c r="F57" s="5">
         <v>14.418147189999999</v>
       </c>
-      <c r="G57" s="5">
+      <c r="G57" s="7">
         <v>0.43213200000000002</v>
       </c>
       <c r="H57" s="5">
@@ -16002,7 +16002,7 @@
       <c r="F58" s="5">
         <v>14.418147189999999</v>
       </c>
-      <c r="G58" s="5">
+      <c r="G58" s="7">
         <v>0.43213200000000002</v>
       </c>
       <c r="H58" s="5">
@@ -16251,7 +16251,7 @@
       <c r="F59" s="5">
         <v>14.418147189999999</v>
       </c>
-      <c r="G59" s="5">
+      <c r="G59" s="7">
         <v>0.43213200000000002</v>
       </c>
       <c r="H59" s="5">
@@ -16500,7 +16500,7 @@
       <c r="F60" s="5">
         <v>14.418147189999999</v>
       </c>
-      <c r="G60" s="5">
+      <c r="G60" s="7">
         <v>0.43213200000000002</v>
       </c>
       <c r="H60" s="5">
@@ -16749,7 +16749,7 @@
       <c r="F61" s="12">
         <v>14.418147189999999</v>
       </c>
-      <c r="G61" s="12">
+      <c r="G61" s="10">
         <v>0.43213200000000002</v>
       </c>
       <c r="H61" s="12">

</xml_diff>

<commit_message>
I am just adding some mean values of NH4 and PO4 for DEMENT
</commit_message>
<xml_diff>
--- a/SP_metadata_2021.xlsx
+++ b/SP_metadata_2021.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugirona-my.sharepoint.com/personal/u4001033_udg_edu/Documents/GRADCATCH/ANALISIS/R/SP_gradient/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\luciana_datos\UCI\Project_14 (Anna)\SP_gradient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="13_ncr:1_{4EEA8018-6EF8-42D3-98FB-882912627FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFE7370F-6C21-40D2-AD8B-D79DB2F6FB54}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F209334-CF43-4E29-B105-1AFA803E0895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP_soil_2021" sheetId="1" r:id="rId1"/>
-    <sheet name="llegenda" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="llegenda" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,36 +72,36 @@
   <commentList>
     <comment ref="E1" authorId="0" shapeId="0" xr:uid="{9D67D6DC-CF53-4FD9-804D-9CAD74BCF708}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Mean Anual Precipitation (mm)
 Extracted by Jonnathan in CLIMATIC_DATA &gt; Results</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1" shapeId="0" xr:uid="{A060A6BB-2CBD-43B3-AC5B-082CEC512E1D}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Mean Anual Temperature (ºC)
 Extracted by Jonnathan in CLIMATIC_DATA &gt; Results</t>
       </text>
     </comment>
     <comment ref="G1" authorId="2" shapeId="0" xr:uid="{B995EEC3-22B8-4EC7-89D8-04467B49E5EA}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Aridity Index
 Extracted by Jonnathan in CLIMATIC_DATA &gt; Results</t>
       </text>
     </comment>
     <comment ref="H1" authorId="3" shapeId="0" xr:uid="{4643F9B3-2625-4E22-B8D3-AEC2801D2687}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Measured in situ (ºC)</t>
       </text>
     </comment>
@@ -158,102 +159,102 @@
     </comment>
     <comment ref="L1" authorId="5" shapeId="0" xr:uid="{3F748EAE-1275-4297-953C-9BFF8326AFE2}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     soil organic matter
 Mean for samples analysed both by Han and me</t>
       </text>
     </comment>
     <comment ref="N1" authorId="6" shapeId="0" xr:uid="{D1572FAE-2DB7-4542-9F5E-D5D55C7DBA14}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Total Organic Carbon (%)</t>
       </text>
     </comment>
     <comment ref="O1" authorId="7" shapeId="0" xr:uid="{9A542229-A5AB-4A4C-8A5E-FAB0986574A7}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Total Carbon (%)</t>
       </text>
     </comment>
     <comment ref="P1" authorId="8" shapeId="0" xr:uid="{856DBA50-38E6-464F-9A04-5AA8CE118D3E}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Total Nitrogen (%)</t>
       </text>
     </comment>
     <comment ref="T1" authorId="9" shapeId="0" xr:uid="{B3BE2832-10E9-440B-AA0D-682097F684C5}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     C/N ratio
 (TC/TN)</t>
       </text>
     </comment>
     <comment ref="U1" authorId="10" shapeId="0" xr:uid="{EC1E8241-F70F-4BE9-B47F-FFBE7926BB63}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     NH4+ (mg/Kg DW soil)</t>
       </text>
     </comment>
     <comment ref="V1" authorId="11" shapeId="0" xr:uid="{1E617BEC-2113-4034-922A-A8AF614A800F}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     PO43-
 (mg/kg DW soil)</t>
       </text>
     </comment>
     <comment ref="W1" authorId="12" shapeId="0" xr:uid="{F3E5E20E-F7AC-40CE-BE07-6D96D6B20EB7}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     SO42-
 (mg/kg DW soil)</t>
       </text>
     </comment>
     <comment ref="AI1" authorId="13" shapeId="0" xr:uid="{A861B59D-14D6-4062-A50E-075AA1D6131B}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Dark CO2 (mmol/m2*d)</t>
       </text>
     </comment>
     <comment ref="AJ1" authorId="14" shapeId="0" xr:uid="{B81A9F97-071D-4C35-895E-BE0BDEE13424}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Light CO2 (mmol/m2*d)</t>
       </text>
     </comment>
     <comment ref="AK1" authorId="15" shapeId="0" xr:uid="{2227ECD2-C3B4-4FD3-9840-F481938E8276}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Average methane values between dark and light
 (umol/m2*d)</t>
       </text>
     </comment>
     <comment ref="AL1" authorId="16" shapeId="0" xr:uid="{CC8F20A9-1D1A-453D-B53F-26E0204A3838}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     (umol/m2*d)</t>
       </text>
     </comment>
@@ -430,54 +431,54 @@
     </comment>
     <comment ref="BB1" authorId="18" shapeId="0" xr:uid="{EFE74430-CE78-45F3-B99F-9E4A66B4DB4A}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     16S rRNA gene
 (copies/g DW soil)</t>
       </text>
     </comment>
     <comment ref="BC1" authorId="19" shapeId="0" xr:uid="{B5AA4312-E55C-4126-AC62-41022648693A}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Fungal ITS2
 (copies/g DW soil)</t>
       </text>
     </comment>
     <comment ref="BG1" authorId="20" shapeId="0" xr:uid="{33824549-3C86-4035-A72B-6643897DCE38}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     arc amoA (AOA)
 (copies/g DW soil)</t>
       </text>
     </comment>
     <comment ref="BH1" authorId="21" shapeId="0" xr:uid="{D4888460-C366-4F77-BB5B-BF617AB9A960}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     bac amoA (AOB)
 (copies/g DW soil)</t>
       </text>
     </comment>
     <comment ref="BJ1" authorId="22" shapeId="0" xr:uid="{97253582-92B4-438A-9794-DF4FB2038D50}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     nosZ Clade I
 (copies/g DW soil)</t>
       </text>
     </comment>
     <comment ref="BL1" authorId="23" shapeId="0" xr:uid="{8F08B99E-9739-4B6E-8F09-DF43B94644DC}">
       <text>
-        <t xml:space="preserve">[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Fluorescence
 Final - Initial
 (nmol raz / gDW*h)
@@ -486,35 +487,35 @@
     </comment>
     <comment ref="BM1" authorId="24" shapeId="0" xr:uid="{B6FFDCB7-FA07-49A4-92C0-69346EC1EFB2}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Bacterial biomass / Fungal biomass
 (mg C / gDW*h)</t>
       </text>
     </comment>
     <comment ref="BN1" authorId="25" shapeId="0" xr:uid="{5E6F31F2-E5EE-4FEA-A394-E8FB2FFDD356}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     16S / ITS2
 (copies / gDW)</t>
       </text>
     </comment>
     <comment ref="BT1" authorId="26" shapeId="0" xr:uid="{C67D560F-8BBA-4DA6-8AE1-F3DD3F0DEC55}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     mg EPS / mg C bact</t>
       </text>
     </comment>
     <comment ref="BX1" authorId="27" shapeId="0" xr:uid="{631D2E3C-FB75-41CC-8E7D-69D20DFEBBF5}">
       <text>
-        <t>[Comentari en fils]
-La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
-Comentari:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     masl</t>
       </text>
     </comment>
@@ -522,8 +523,55 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={4081FDEB-35DC-4D72-B8D0-0F29840F5E80}</author>
+    <author>tc={A17C3618-9073-47D4-A8FB-C2BAC082C93C}</author>
+    <author>tc={B07C916B-4DC3-40A8-9BF7-5FBA1D7F0473}</author>
+    <author>tc={FE35A6FF-3B2A-4AE9-85C1-0C9D805121A4}</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{4081FDEB-35DC-4D72-B8D0-0F29840F5E80}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NH4+ (mg/Kg DW soil)</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{A17C3618-9073-47D4-A8FB-C2BAC082C93C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PO43-
+(mg/kg DW soil)</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="2" shapeId="0" xr:uid="{B07C916B-4DC3-40A8-9BF7-5FBA1D7F0473}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NH4+ (mg/Kg DW soil)</t>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="3" shapeId="0" xr:uid="{FE35A6FF-3B2A-4AE9-85C1-0C9D805121A4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PO43-
+(mg/kg DW soil)</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="234">
   <si>
     <t>1-SP01-A</t>
   </si>
@@ -1260,7 +1308,7 @@
     <numFmt numFmtId="167" formatCode="0.00000"/>
     <numFmt numFmtId="168" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1292,6 +1340,18 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1386,7 +1446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1502,6 +1562,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1912,15 +1977,34 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2023-03-01T13:41:18.13" personId="{5C2DB10E-6B8E-4F59-90D1-A869F7498523}" id="{4081FDEB-35DC-4D72-B8D0-0F29840F5E80}">
+    <text>NH4+ (mg/Kg DW soil)</text>
+  </threadedComment>
+  <threadedComment ref="E1" dT="2023-03-01T14:05:34.86" personId="{5C2DB10E-6B8E-4F59-90D1-A869F7498523}" id="{A17C3618-9073-47D4-A8FB-C2BAC082C93C}">
+    <text>PO43-
+(mg/kg DW soil)</text>
+  </threadedComment>
+  <threadedComment ref="I1" dT="2023-03-01T13:41:18.13" personId="{5C2DB10E-6B8E-4F59-90D1-A869F7498523}" id="{B07C916B-4DC3-40A8-9BF7-5FBA1D7F0473}">
+    <text>NH4+ (mg/Kg DW soil)</text>
+  </threadedComment>
+  <threadedComment ref="J1" dT="2023-03-01T14:05:34.86" personId="{5C2DB10E-6B8E-4F59-90D1-A869F7498523}" id="{FE35A6FF-3B2A-4AE9-85C1-0C9D805121A4}">
+    <text>PO43-
+(mg/kg DW soil)</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CN61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W23" sqref="W23"/>
+      <selection pane="bottomRight" activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19344,11 +19428,653 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD626EB-9DDD-4FC9-BAF5-409CC1F59D7A}">
+  <dimension ref="C1:J51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C1" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="7">
+        <v>10.79</v>
+      </c>
+      <c r="E2" s="1">
+        <v>11.35</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="39">
+        <f>AVERAGE(D2:D6)</f>
+        <v>12.007999999999999</v>
+      </c>
+      <c r="J2" s="39">
+        <f>AVERAGE(E2:E6)</f>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="7">
+        <v>31.01</v>
+      </c>
+      <c r="E3" s="1">
+        <v>17.47</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="39">
+        <f>AVERAGE(D7:D11)</f>
+        <v>33.962000000000003</v>
+      </c>
+      <c r="J3" s="39">
+        <f>AVERAGE(E7:E11)</f>
+        <v>119.94800000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="7">
+        <v>6.59</v>
+      </c>
+      <c r="E4" s="1">
+        <v>16.14</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="39">
+        <f>AVERAGE(D12:D16)</f>
+        <v>30.32</v>
+      </c>
+      <c r="J4" s="39">
+        <f>AVERAGE(E12:E16)</f>
+        <v>5.194</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="7">
+        <v>5.46</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6.61</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="39">
+        <f>AVERAGE(D17:D21)</f>
+        <v>4.9760000000000009</v>
+      </c>
+      <c r="J5" s="39">
+        <f>AVERAGE(E17:E21)</f>
+        <v>23.824000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="7">
+        <v>6.19</v>
+      </c>
+      <c r="E6" s="1">
+        <v>12.93</v>
+      </c>
+      <c r="H6" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="39">
+        <f>AVERAGE(D22:D26)</f>
+        <v>49.1</v>
+      </c>
+      <c r="J6" s="39">
+        <f>AVERAGE(E22:E26)</f>
+        <v>5.0539999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="7">
+        <v>66.84</v>
+      </c>
+      <c r="E7" s="1">
+        <v>84.42</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="7">
+        <v>7.07</v>
+      </c>
+      <c r="E8" s="1">
+        <v>158.78</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="7">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E9" s="1">
+        <v>112.02</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="7">
+        <v>79.37</v>
+      </c>
+      <c r="E10" s="1">
+        <v>143.31</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="7">
+        <v>7.33</v>
+      </c>
+      <c r="E11" s="1">
+        <v>101.21</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="7">
+        <v>13.75</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="7">
+        <v>7.49</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="7">
+        <v>30.57</v>
+      </c>
+      <c r="E14" s="1">
+        <v>10.79</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="7">
+        <v>94.7</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="7">
+        <v>5.09</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="7">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="E17" s="1">
+        <v>20.079999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="7">
+        <v>5.34</v>
+      </c>
+      <c r="E18" s="1">
+        <v>34.96</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="7">
+        <v>5.33</v>
+      </c>
+      <c r="E19" s="1">
+        <v>23.37</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="7">
+        <v>4.46</v>
+      </c>
+      <c r="E20" s="1">
+        <v>16.59</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="7">
+        <v>5.6</v>
+      </c>
+      <c r="E21" s="1">
+        <v>24.12</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="7">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="E22" s="1">
+        <v>6.04</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="7">
+        <v>6.22</v>
+      </c>
+      <c r="E23" s="1">
+        <v>4.7699999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="7">
+        <v>169.5</v>
+      </c>
+      <c r="E24" s="1">
+        <v>6.04</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="7">
+        <v>60.66</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="7">
+        <v>4.76</v>
+      </c>
+      <c r="E26" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="7">
+        <v>46.46</v>
+      </c>
+      <c r="E27" s="1">
+        <v>44.45</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="7">
+        <v>85.05</v>
+      </c>
+      <c r="E28" s="1">
+        <v>64.91</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="7">
+        <v>304.72000000000003</v>
+      </c>
+      <c r="E29" s="1">
+        <v>77.02</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="7">
+        <v>86.35</v>
+      </c>
+      <c r="E30" s="1">
+        <v>67.400000000000006</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="7">
+        <v>119.14</v>
+      </c>
+      <c r="E31" s="1">
+        <v>62.11</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="7">
+        <v>24.71</v>
+      </c>
+      <c r="E32" s="1">
+        <v>17.420000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="7">
+        <v>59.67</v>
+      </c>
+      <c r="E33" s="1">
+        <v>27.47</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="7">
+        <v>44.4</v>
+      </c>
+      <c r="E34" s="1">
+        <v>34.049999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="7">
+        <v>35.130000000000003</v>
+      </c>
+      <c r="E35" s="1">
+        <v>21.83</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="7">
+        <v>27.94</v>
+      </c>
+      <c r="E36" s="1">
+        <v>11.73</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="7">
+        <v>13.94</v>
+      </c>
+      <c r="E37" s="1">
+        <v>27.56</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="7">
+        <v>19.78</v>
+      </c>
+      <c r="E38" s="1">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="7">
+        <v>31</v>
+      </c>
+      <c r="E39" s="1">
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="7">
+        <v>14.39</v>
+      </c>
+      <c r="E40" s="1">
+        <v>26.94</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="7">
+        <v>16.079999999999998</v>
+      </c>
+      <c r="E41" s="1">
+        <v>24.69</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="7">
+        <v>73.75</v>
+      </c>
+      <c r="E42" s="1">
+        <v>6.51</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="7">
+        <v>5.25</v>
+      </c>
+      <c r="E43" s="1">
+        <v>6.03</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="7">
+        <v>4.67</v>
+      </c>
+      <c r="E44" s="1">
+        <v>7.85</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" s="7">
+        <v>3.8</v>
+      </c>
+      <c r="E45" s="1">
+        <v>5.96</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D46" s="7">
+        <v>4.37</v>
+      </c>
+      <c r="E46" s="1">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C47" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" s="7">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="E47" s="1">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C48" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" s="7">
+        <v>44.44</v>
+      </c>
+      <c r="E48" s="1">
+        <v>4.96</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="7">
+        <v>33.07</v>
+      </c>
+      <c r="E49" s="1">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" s="7">
+        <v>32.57</v>
+      </c>
+      <c r="E50" s="1">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" s="7">
+        <v>31.21</v>
+      </c>
+      <c r="E51" s="1">
+        <v>4.03</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2851FD1-392A-48A9-B131-D748FDC4A90A}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
actualized plots, new mantel tests
</commit_message>
<xml_diff>
--- a/SP_metadata_2021.xlsx
+++ b/SP_metadata_2021.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\luciana_datos\UCI\Project_14 (Anna)\SP_gradient\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugirona-my.sharepoint.com/personal/u4001033_udg_edu/Documents/GRADCATCH/ANALISIS/R/SP_gradient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA000A84-3FBB-4950-9B47-833BA501E91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{CA000A84-3FBB-4950-9B47-833BA501E91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96F7789D-AC30-4DD5-94F5-D5E6AA4439DB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP_soil_2021" sheetId="1" r:id="rId1"/>
-    <sheet name="llegenda" sheetId="2" r:id="rId2"/>
+    <sheet name="Full1" sheetId="3" r:id="rId2"/>
+    <sheet name="llegenda" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,36 +72,36 @@
   <commentList>
     <comment ref="E1" authorId="0" shapeId="0" xr:uid="{9D67D6DC-CF53-4FD9-804D-9CAD74BCF708}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Mean Anual Precipitation (mm)
 Extracted by Jonnathan in CLIMATIC_DATA &gt; Results</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1" shapeId="0" xr:uid="{A060A6BB-2CBD-43B3-AC5B-082CEC512E1D}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Mean Anual Temperature (ºC)
 Extracted by Jonnathan in CLIMATIC_DATA &gt; Results</t>
       </text>
     </comment>
     <comment ref="G1" authorId="2" shapeId="0" xr:uid="{B995EEC3-22B8-4EC7-89D8-04467B49E5EA}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Aridity Index
 Extracted by Jonnathan in CLIMATIC_DATA &gt; Results</t>
       </text>
     </comment>
     <comment ref="H1" authorId="3" shapeId="0" xr:uid="{4643F9B3-2625-4E22-B8D3-AEC2801D2687}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Measured in situ (ºC)</t>
       </text>
     </comment>
@@ -158,102 +159,102 @@
     </comment>
     <comment ref="L1" authorId="5" shapeId="0" xr:uid="{3F748EAE-1275-4297-953C-9BFF8326AFE2}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     soil organic matter
 Mean for samples analysed both by Han and me</t>
       </text>
     </comment>
     <comment ref="N1" authorId="6" shapeId="0" xr:uid="{D1572FAE-2DB7-4542-9F5E-D5D55C7DBA14}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Total Organic Carbon (%)</t>
       </text>
     </comment>
     <comment ref="O1" authorId="7" shapeId="0" xr:uid="{9A542229-A5AB-4A4C-8A5E-FAB0986574A7}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Total Carbon (%)</t>
       </text>
     </comment>
     <comment ref="P1" authorId="8" shapeId="0" xr:uid="{856DBA50-38E6-464F-9A04-5AA8CE118D3E}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Total Nitrogen (%)</t>
       </text>
     </comment>
     <comment ref="T1" authorId="9" shapeId="0" xr:uid="{B3BE2832-10E9-440B-AA0D-682097F684C5}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     C/N ratio
 (TC/TN)</t>
       </text>
     </comment>
     <comment ref="U1" authorId="10" shapeId="0" xr:uid="{EC1E8241-F70F-4BE9-B47F-FFBE7926BB63}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     NH4+ (mg/Kg DW soil)</t>
       </text>
     </comment>
     <comment ref="V1" authorId="11" shapeId="0" xr:uid="{1E617BEC-2113-4034-922A-A8AF614A800F}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     PO43-
 (mg/kg DW soil)</t>
       </text>
     </comment>
     <comment ref="W1" authorId="12" shapeId="0" xr:uid="{F3E5E20E-F7AC-40CE-BE07-6D96D6B20EB7}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     SO42-
 (mg/kg DW soil)</t>
       </text>
     </comment>
     <comment ref="AI1" authorId="13" shapeId="0" xr:uid="{A861B59D-14D6-4062-A50E-075AA1D6131B}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Dark CO2 (mmol/m2*d)</t>
       </text>
     </comment>
     <comment ref="AJ1" authorId="14" shapeId="0" xr:uid="{B81A9F97-071D-4C35-895E-BE0BDEE13424}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Light CO2 (mmol/m2*d)</t>
       </text>
     </comment>
     <comment ref="AK1" authorId="15" shapeId="0" xr:uid="{2227ECD2-C3B4-4FD3-9840-F481938E8276}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Average methane values between dark and light
 (umol/m2*d)</t>
       </text>
     </comment>
     <comment ref="AL1" authorId="16" shapeId="0" xr:uid="{CC8F20A9-1D1A-453D-B53F-26E0204A3838}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     (umol/m2*d)</t>
       </text>
     </comment>
@@ -430,54 +431,54 @@
     </comment>
     <comment ref="BB1" authorId="18" shapeId="0" xr:uid="{EFE74430-CE78-45F3-B99F-9E4A66B4DB4A}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     16S rRNA gene
 (copies/g DW soil)</t>
       </text>
     </comment>
     <comment ref="BC1" authorId="19" shapeId="0" xr:uid="{B5AA4312-E55C-4126-AC62-41022648693A}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Fungal ITS2
 (copies/g DW soil)</t>
       </text>
     </comment>
     <comment ref="BG1" authorId="20" shapeId="0" xr:uid="{33824549-3C86-4035-A72B-6643897DCE38}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     arc amoA (AOA)
 (copies/g DW soil)</t>
       </text>
     </comment>
     <comment ref="BH1" authorId="21" shapeId="0" xr:uid="{D4888460-C366-4F77-BB5B-BF617AB9A960}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     bac amoA (AOB)
 (copies/g DW soil)</t>
       </text>
     </comment>
     <comment ref="BJ1" authorId="22" shapeId="0" xr:uid="{97253582-92B4-438A-9794-DF4FB2038D50}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     nosZ Clade I
 (copies/g DW soil)</t>
       </text>
     </comment>
     <comment ref="BL1" authorId="23" shapeId="0" xr:uid="{8F08B99E-9739-4B6E-8F09-DF43B94644DC}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t xml:space="preserve">[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Fluorescence
 Final - Initial
 (nmol raz / gDW*h)
@@ -486,35 +487,35 @@
     </comment>
     <comment ref="BM1" authorId="24" shapeId="0" xr:uid="{B6FFDCB7-FA07-49A4-92C0-69346EC1EFB2}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     Bacterial biomass / Fungal biomass
 (mg C / gDW*h)</t>
       </text>
     </comment>
     <comment ref="BN1" authorId="25" shapeId="0" xr:uid="{5E6F31F2-E5EE-4FEA-A394-E8FB2FFDD356}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     16S / ITS2
 (copies / gDW)</t>
       </text>
     </comment>
     <comment ref="BT1" authorId="26" shapeId="0" xr:uid="{C67D560F-8BBA-4DA6-8AE1-F3DD3F0DEC55}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     mg EPS / mg C bact</t>
       </text>
     </comment>
     <comment ref="BX1" authorId="27" shapeId="0" xr:uid="{631D2E3C-FB75-41CC-8E7D-69D20DFEBBF5}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentari en fils]
+La vostra versió de l'Excel us permet llegir aquest comentari en fils. No obstant això, les edicions que s'hi apliquin se suprimiran si el fitxer s'obre en una versió més recent de l'Excel. Més informació: https://go.microsoft.com/fwlink/?linkid=870924.
+Comentari:
     masl</t>
       </text>
     </comment>
@@ -523,7 +524,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="237">
   <si>
     <t>1-SP01-A</t>
   </si>
@@ -1248,17 +1249,27 @@
   <si>
     <t>HIX</t>
   </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000000"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
     <numFmt numFmtId="168" formatCode="0.0000000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1386,7 +1397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1502,6 +1513,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1916,11 +1929,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CN61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z17" sqref="Z17"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="1" sqref="M1:M1048576 B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19344,6 +19357,814 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEFF931-4757-4988-B960-6E1121EFFF96}">
+  <dimension ref="A1:E62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="5">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="C2" s="39">
+        <f>AVERAGE(B2:B6)</f>
+        <v>4.3160000000000007</v>
+      </c>
+      <c r="D2" s="39">
+        <f>_xlfn.STDEV.S(B2:B6)</f>
+        <v>0.15043270920913462</v>
+      </c>
+      <c r="E2" s="40">
+        <f>D2/SQRT(5)</f>
+        <v>6.7275552766216731E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="5">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="5">
+        <v>4.34</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="5">
+        <v>4.53</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="40"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4.21</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="5">
+        <v>4.16</v>
+      </c>
+      <c r="C7" s="39">
+        <f>AVERAGE(B7:B11)</f>
+        <v>4.452</v>
+      </c>
+      <c r="D7" s="39">
+        <f>_xlfn.STDEV.S(B7:B11)</f>
+        <v>0.39505695791872836</v>
+      </c>
+      <c r="E7" s="40">
+        <f>D7/SQRT(5)</f>
+        <v>0.17667484257811009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="5">
+        <v>4.54</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="40"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4.45</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="40"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="5">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="40"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="5">
+        <v>4.05</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="40"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="5">
+        <v>4.97</v>
+      </c>
+      <c r="C12" s="39">
+        <f>AVERAGE(B12:B16)</f>
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="D12" s="39">
+        <f>_xlfn.STDEV.S(B12:B16)</f>
+        <v>0.29094673051952313</v>
+      </c>
+      <c r="E12" s="40">
+        <f>D12/SQRT(5)</f>
+        <v>0.13011533345459328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="5">
+        <v>4.43</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="40"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="5">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="5">
+        <v>4.87</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="5">
+        <v>7.74</v>
+      </c>
+      <c r="C17" s="39">
+        <f>AVERAGE(B17:B21)</f>
+        <v>7.548</v>
+      </c>
+      <c r="D17" s="39">
+        <f>_xlfn.STDEV.S(B17:B21)</f>
+        <v>0.12794530081249567</v>
+      </c>
+      <c r="E17" s="40">
+        <f>D17/SQRT(5)</f>
+        <v>5.7218878003679877E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="5">
+        <v>7.4</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="5">
+        <v>7.56</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="40"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="5">
+        <v>7.57</v>
+      </c>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="40"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="5">
+        <v>7.47</v>
+      </c>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="40"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="5">
+        <v>7.68</v>
+      </c>
+      <c r="C22" s="39">
+        <f>AVERAGE(B22:B26)</f>
+        <v>7.7120000000000006</v>
+      </c>
+      <c r="D22" s="39">
+        <f>_xlfn.STDEV.S(B22:B26)</f>
+        <v>3.7013511046643549E-2</v>
+      </c>
+      <c r="E22" s="40">
+        <f>D22/SQRT(5)</f>
+        <v>1.655294535724687E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="5">
+        <v>7.76</v>
+      </c>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="40"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="5">
+        <v>7.67</v>
+      </c>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="40"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="5">
+        <v>7.73</v>
+      </c>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="40"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="5">
+        <v>7.72</v>
+      </c>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="40"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="5">
+        <v>6.24</v>
+      </c>
+      <c r="C27" s="39">
+        <f>AVERAGE(B27:B31)</f>
+        <v>6.1180000000000003</v>
+      </c>
+      <c r="D27" s="39">
+        <f>_xlfn.STDEV.S(B27:B31)</f>
+        <v>0.21040437257813846</v>
+      </c>
+      <c r="E27" s="40">
+        <f>D27/SQRT(5)</f>
+        <v>9.4095695969582047E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="5">
+        <v>5.89</v>
+      </c>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="40"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="5">
+        <v>6.25</v>
+      </c>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="40"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="5">
+        <v>5.89</v>
+      </c>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="40"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="5">
+        <v>6.32</v>
+      </c>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="40"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="5">
+        <v>4.53</v>
+      </c>
+      <c r="C32" s="39">
+        <f>AVERAGE(B32:B36)</f>
+        <v>4.2219999999999995</v>
+      </c>
+      <c r="D32" s="39">
+        <f>_xlfn.STDEV.S(B32:B36)</f>
+        <v>0.3131613002910803</v>
+      </c>
+      <c r="E32" s="40">
+        <f>D32/SQRT(5)</f>
+        <v>0.14004999107461605</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="5">
+        <v>4.53</v>
+      </c>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="40"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="5">
+        <v>4.21</v>
+      </c>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="40"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="5">
+        <v>3.82</v>
+      </c>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="40"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="5">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="40"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="5">
+        <v>3.89</v>
+      </c>
+      <c r="C37" s="39">
+        <f>AVERAGE(B37:B41)</f>
+        <v>3.778</v>
+      </c>
+      <c r="D37" s="39">
+        <f>_xlfn.STDEV.S(B37:B41)</f>
+        <v>0.1492313639956428</v>
+      </c>
+      <c r="E37" s="40">
+        <f>D37/SQRT(5)</f>
+        <v>6.673829485385438E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="5">
+        <v>3.93</v>
+      </c>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="40"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="5">
+        <v>3.78</v>
+      </c>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="40"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="5">
+        <v>3.55</v>
+      </c>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="40"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="5">
+        <v>3.74</v>
+      </c>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="40"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="5">
+        <v>7.53</v>
+      </c>
+      <c r="C42" s="39">
+        <f>AVERAGE(B42:B46)</f>
+        <v>7.6020000000000012</v>
+      </c>
+      <c r="D42" s="39">
+        <f>_xlfn.STDEV.S(B42:B46)</f>
+        <v>6.6105975524153551E-2</v>
+      </c>
+      <c r="E42" s="40">
+        <f>D42/SQRT(5)</f>
+        <v>2.9563490998188925E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="5">
+        <v>7.64</v>
+      </c>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="40"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="5">
+        <v>7.53</v>
+      </c>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="40"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="5">
+        <v>7.65</v>
+      </c>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="40"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="5">
+        <v>7.66</v>
+      </c>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="40"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="5">
+        <v>7.72</v>
+      </c>
+      <c r="C47" s="39">
+        <f>AVERAGE(B47:B51)</f>
+        <v>7.694</v>
+      </c>
+      <c r="D47" s="39">
+        <f>_xlfn.STDEV.S(B47:B51)</f>
+        <v>5.4589376255824565E-2</v>
+      </c>
+      <c r="E47" s="40">
+        <f>D47/SQRT(5)</f>
+        <v>2.4413111231467333E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="5">
+        <v>7.62</v>
+      </c>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="40"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="5">
+        <v>7.76</v>
+      </c>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="40"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="5">
+        <v>7.71</v>
+      </c>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="40"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="5">
+        <v>7.66</v>
+      </c>
+      <c r="C51" s="39"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="40"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="5">
+        <v>7.28</v>
+      </c>
+      <c r="C52" s="39">
+        <f>AVERAGE(B52:B56)</f>
+        <v>7.0920000000000005</v>
+      </c>
+      <c r="D52" s="39">
+        <f>_xlfn.STDEV.S(B52:B56)</f>
+        <v>0.3002831996632514</v>
+      </c>
+      <c r="E52" s="40">
+        <f>D52/SQRT(5)</f>
+        <v>0.13429072938963441</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="5">
+        <v>7.09</v>
+      </c>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="40"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="5">
+        <v>7.38</v>
+      </c>
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="40"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="5">
+        <v>6.6</v>
+      </c>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="40"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" s="5">
+        <v>7.11</v>
+      </c>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="40"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="5">
+        <v>5.99</v>
+      </c>
+      <c r="C57" s="39">
+        <f>AVERAGE(B57:B61)</f>
+        <v>5.6419999999999995</v>
+      </c>
+      <c r="D57" s="39">
+        <f>_xlfn.STDEV.S(B57:B61)</f>
+        <v>0.33417061510551754</v>
+      </c>
+      <c r="E57" s="40">
+        <f>D57/SQRT(5)</f>
+        <v>0.14944564229177104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="5">
+        <v>5.79</v>
+      </c>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="40"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B59" s="5">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="C59" s="39"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="40"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B60" s="5">
+        <v>5.76</v>
+      </c>
+      <c r="C60" s="39"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="40"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" s="12">
+        <v>5.56</v>
+      </c>
+      <c r="C61" s="39"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="40"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2851FD1-392A-48A9-B131-D748FDC4A90A}">
   <dimension ref="A1:A3"/>
   <sheetViews>

</xml_diff>